<commit_message>
fix: bug save load
</commit_message>
<xml_diff>
--- a/data/en-us/talents.xlsx
+++ b/data/en-us/talents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84694\Desktop\人生重来\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DE8C90-6419-47E8-B9C6-ECA6A96A2FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAA4FEF-93F8-469F-A8CD-2ABDF334A9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="585">
   <si>
     <t>序号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2265,6 +2265,22 @@
   </si>
   <si>
     <t>得过诺贝尔奖可复活一次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>加一条命</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>死者苏生</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有属性-2，加一条命</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>恶魔的交易</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2669,13 +2685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL184"/>
+  <dimension ref="A1:AL186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D162" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D149" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H168" sqref="H168"/>
+      <selection pane="bottomRight" activeCell="C150" sqref="A149:C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5" defaultRowHeight="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5762,87 +5778,96 @@
     </row>
     <row r="149" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>2001</v>
+        <v>1147</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>509</v>
+        <v>582</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>510</v>
+        <v>581</v>
       </c>
       <c r="E149" s="1">
-        <v>2</v>
-      </c>
-      <c r="F149" s="1">
-        <v>1</v>
-      </c>
-      <c r="K149" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>2002</v>
+        <v>1148</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>511</v>
+        <v>584</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>512</v>
+        <v>583</v>
       </c>
       <c r="E150" s="1">
         <v>2</v>
       </c>
-      <c r="F150" s="1">
-        <v>1</v>
+      <c r="H150" s="1">
+        <v>-2</v>
+      </c>
+      <c r="I150" s="1">
+        <v>-2</v>
       </c>
       <c r="J150" s="1">
-        <v>4</v>
+        <v>-2</v>
+      </c>
+      <c r="K150" s="1">
+        <v>-2</v>
+      </c>
+      <c r="L150" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="151" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="E151" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F151" s="1">
         <v>1</v>
+      </c>
+      <c r="K151" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="E152" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F152" s="1">
         <v>1</v>
+      </c>
+      <c r="J152" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="C153" s="1">
-        <v>3.1415926000000001</v>
+        <v>514</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>513</v>
       </c>
       <c r="E153" s="1">
         <v>0</v>
@@ -5853,83 +5878,41 @@
     </row>
     <row r="154" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E154" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F154" s="1">
         <v>1</v>
-      </c>
-      <c r="N154" s="1">
-        <v>2</v>
-      </c>
-      <c r="AE154" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="AF154" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="AG154" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="AH154" s="1">
-        <v>1110</v>
-      </c>
-      <c r="AI154" s="1">
-        <v>1003</v>
-      </c>
-      <c r="AJ154" s="1">
-        <v>1004</v>
-      </c>
-      <c r="AK154" s="1">
-        <v>1124</v>
-      </c>
-      <c r="AL154" s="1">
-        <v>1125</v>
       </c>
     </row>
     <row r="155" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>328</v>
+        <v>519</v>
+      </c>
+      <c r="C155" s="1">
+        <v>3.1415926000000001</v>
       </c>
       <c r="E155" s="1">
         <v>0</v>
       </c>
       <c r="F155" s="1">
-        <v>1</v>
-      </c>
-      <c r="H155" s="1">
-        <v>1</v>
-      </c>
-      <c r="I155" s="1">
-        <v>1</v>
-      </c>
-      <c r="J155" s="1">
-        <v>1</v>
-      </c>
-      <c r="L155" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>521</v>
@@ -5937,40 +5920,52 @@
       <c r="C156" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D156" s="5" t="s">
-        <v>354</v>
-      </c>
       <c r="E156" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F156" s="1">
         <v>1</v>
       </c>
-      <c r="H156" s="1">
-        <v>1</v>
-      </c>
-      <c r="I156" s="1">
-        <v>1</v>
-      </c>
-      <c r="J156" s="1">
-        <v>1</v>
-      </c>
-      <c r="K156" s="1">
-        <v>1</v>
-      </c>
-      <c r="L156" s="1">
-        <v>1</v>
+      <c r="N156" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE156" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="AF156" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="AG156" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="AH156" s="1">
+        <v>1110</v>
+      </c>
+      <c r="AI156" s="1">
+        <v>1003</v>
+      </c>
+      <c r="AJ156" s="1">
+        <v>1004</v>
+      </c>
+      <c r="AK156" s="1">
+        <v>1124</v>
+      </c>
+      <c r="AL156" s="1">
+        <v>1125</v>
       </c>
     </row>
     <row r="157" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="E157" s="1">
         <v>0</v>
@@ -5978,43 +5973,31 @@
       <c r="F157" s="1">
         <v>1</v>
       </c>
-      <c r="N157" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE157" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="AF157" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="AG157" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="AH157" s="1">
-        <v>1110</v>
-      </c>
-      <c r="AI157" s="1">
-        <v>1003</v>
-      </c>
-      <c r="AJ157" s="1">
-        <v>1004</v>
-      </c>
-      <c r="AK157" s="1">
-        <v>1124</v>
-      </c>
-      <c r="AL157" s="1">
-        <v>1125</v>
+      <c r="H157" s="1">
+        <v>1</v>
+      </c>
+      <c r="I157" s="1">
+        <v>1</v>
+      </c>
+      <c r="J157" s="1">
+        <v>1</v>
+      </c>
+      <c r="L157" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>354</v>
       </c>
       <c r="E158" s="1">
         <v>0</v>
@@ -6022,37 +6005,25 @@
       <c r="F158" s="1">
         <v>1</v>
       </c>
-      <c r="N158" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE158" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="AF158" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="AG158" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="AH158" s="1">
-        <v>1110</v>
-      </c>
-      <c r="AI158" s="1">
-        <v>1003</v>
-      </c>
-      <c r="AJ158" s="1">
-        <v>1004</v>
-      </c>
-      <c r="AK158" s="1">
-        <v>1124</v>
-      </c>
-      <c r="AL158" s="1">
-        <v>1125</v>
+      <c r="H158" s="1">
+        <v>1</v>
+      </c>
+      <c r="I158" s="1">
+        <v>1</v>
+      </c>
+      <c r="J158" s="1">
+        <v>1</v>
+      </c>
+      <c r="K158" s="1">
+        <v>1</v>
+      </c>
+      <c r="L158" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>522</v>
@@ -6096,7 +6067,7 @@
     </row>
     <row r="160" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>522</v>
@@ -6140,7 +6111,7 @@
     </row>
     <row r="161" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>522</v>
@@ -6184,169 +6155,211 @@
     </row>
     <row r="162" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E162" s="1">
         <v>0</v>
       </c>
       <c r="F162" s="1">
         <v>1</v>
+      </c>
+      <c r="N162" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE162" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="AF162" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="AG162" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="AH162" s="1">
+        <v>1110</v>
+      </c>
+      <c r="AI162" s="1">
+        <v>1003</v>
+      </c>
+      <c r="AJ162" s="1">
+        <v>1004</v>
+      </c>
+      <c r="AK162" s="1">
+        <v>1124</v>
+      </c>
+      <c r="AL162" s="1">
+        <v>1125</v>
       </c>
     </row>
     <row r="163" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="E163" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F163" s="1">
         <v>1</v>
       </c>
-      <c r="G163" s="1">
-        <v>1</v>
-      </c>
-      <c r="H163" s="1">
-        <v>5</v>
-      </c>
-      <c r="I163" s="1">
-        <v>1</v>
-      </c>
-      <c r="J163" s="1">
-        <v>1</v>
-      </c>
-      <c r="K163" s="1">
-        <v>2</v>
-      </c>
-      <c r="L163" s="1">
-        <v>1</v>
-      </c>
-      <c r="M163" s="1">
-        <v>1</v>
+      <c r="N163" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE163" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="AF163" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="AG163" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="AH163" s="1">
+        <v>1110</v>
+      </c>
+      <c r="AI163" s="1">
+        <v>1003</v>
+      </c>
+      <c r="AJ163" s="1">
+        <v>1004</v>
+      </c>
+      <c r="AK163" s="1">
+        <v>1124</v>
+      </c>
+      <c r="AL163" s="1">
+        <v>1125</v>
       </c>
     </row>
     <row r="164" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="E164" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F164" s="1">
         <v>1</v>
-      </c>
-      <c r="O164" s="1">
-        <v>1141</v>
-      </c>
-      <c r="P164" s="1">
-        <v>1135</v>
-      </c>
-      <c r="Q164" s="1">
-        <v>1114</v>
-      </c>
-      <c r="R164" s="1">
-        <v>1023</v>
-      </c>
-      <c r="S164" s="1">
-        <v>1048</v>
-      </c>
-      <c r="T164" s="1" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="165" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="E165" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F165" s="1">
+        <v>1</v>
+      </c>
+      <c r="G165" s="1">
+        <v>1</v>
+      </c>
+      <c r="H165" s="1">
+        <v>5</v>
+      </c>
+      <c r="I165" s="1">
+        <v>1</v>
+      </c>
+      <c r="J165" s="1">
+        <v>1</v>
+      </c>
+      <c r="K165" s="1">
+        <v>2</v>
+      </c>
+      <c r="L165" s="1">
+        <v>1</v>
+      </c>
+      <c r="M165" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>363</v>
+        <v>529</v>
       </c>
       <c r="E166" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F166" s="1">
         <v>1</v>
       </c>
-      <c r="K166" s="1">
-        <v>-2</v>
+      <c r="O166" s="1">
+        <v>1141</v>
+      </c>
+      <c r="P166" s="1">
+        <v>1135</v>
+      </c>
+      <c r="Q166" s="1">
+        <v>1114</v>
+      </c>
+      <c r="R166" s="1">
+        <v>1023</v>
+      </c>
+      <c r="S166" s="1">
+        <v>1048</v>
+      </c>
+      <c r="T166" s="1" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="167" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>498</v>
+        <v>533</v>
       </c>
       <c r="E167" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F167" s="1">
         <v>1</v>
-      </c>
-      <c r="I167" s="1">
-        <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>538</v>
+        <v>363</v>
       </c>
       <c r="E168" s="1">
         <v>0</v>
@@ -6354,115 +6367,127 @@
       <c r="F168" s="1">
         <v>1</v>
       </c>
-      <c r="J168" s="1">
+      <c r="K168" s="1">
         <v>-2</v>
       </c>
     </row>
     <row r="169" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>540</v>
+        <v>535</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>498</v>
       </c>
       <c r="E169" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F169" s="1">
         <v>1</v>
       </c>
-      <c r="O169" s="6" t="s">
-        <v>541</v>
-      </c>
-      <c r="P169" s="6" t="s">
-        <v>542</v>
-      </c>
-      <c r="Q169" s="6" t="s">
-        <v>543</v>
-      </c>
-      <c r="R169" s="6" t="s">
-        <v>544</v>
-      </c>
-      <c r="S169" s="6" t="s">
-        <v>545</v>
-      </c>
-      <c r="T169" s="6" t="s">
-        <v>546</v>
-      </c>
-      <c r="U169" s="6" t="s">
-        <v>547</v>
-      </c>
-      <c r="V169" s="6" t="s">
-        <v>548</v>
-      </c>
-      <c r="W169" s="6" t="s">
-        <v>549</v>
-      </c>
-      <c r="X169" s="6" t="s">
-        <v>550</v>
-      </c>
-      <c r="Y169" s="6" t="s">
-        <v>551</v>
-      </c>
-      <c r="Z169" s="6" t="s">
-        <v>552</v>
-      </c>
-      <c r="AA169" s="6" t="s">
-        <v>553</v>
-      </c>
-      <c r="AB169" s="6"/>
-      <c r="AC169" s="6"/>
-      <c r="AD169" s="6"/>
+      <c r="I169" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="170" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>554</v>
+        <v>536</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>555</v>
+        <v>537</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>538</v>
       </c>
       <c r="E170" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F170" s="1">
         <v>1</v>
+      </c>
+      <c r="J170" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="171" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>556</v>
+        <v>539</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>557</v>
+        <v>540</v>
       </c>
       <c r="E171" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F171" s="1">
         <v>1</v>
       </c>
+      <c r="O171" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="P171" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q171" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="R171" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="S171" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="T171" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="U171" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="V171" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="W171" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="X171" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="Y171" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="Z171" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="AA171" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="AB171" s="6"/>
+      <c r="AC171" s="6"/>
+      <c r="AD171" s="6"/>
     </row>
     <row r="172" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>580</v>
+        <v>555</v>
       </c>
       <c r="E172" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F172" s="1">
         <v>1</v>
@@ -6470,149 +6495,143 @@
     </row>
     <row r="173" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>478</v>
+        <v>557</v>
       </c>
       <c r="E173" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F173" s="1">
         <v>1</v>
-      </c>
-      <c r="N173" s="1">
-        <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>564</v>
+        <v>580</v>
       </c>
       <c r="E174" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F174" s="1">
-        <v>1</v>
-      </c>
-      <c r="H174" s="1">
-        <v>1</v>
-      </c>
-      <c r="I174" s="1">
-        <v>1</v>
-      </c>
-      <c r="J174" s="1">
-        <v>1</v>
-      </c>
-      <c r="K174" s="1">
-        <v>1</v>
-      </c>
-      <c r="L174" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>561</v>
+        <v>478</v>
       </c>
       <c r="E175" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F175" s="1">
         <v>1</v>
       </c>
-      <c r="O175" s="1">
-        <v>2028</v>
-      </c>
-      <c r="P175" s="1">
-        <v>2029</v>
-      </c>
-      <c r="Q175" s="1">
-        <v>2030</v>
-      </c>
-      <c r="R175" s="1">
-        <v>2031</v>
-      </c>
-      <c r="S175" s="1">
-        <v>2032</v>
-      </c>
-      <c r="T175" s="1">
-        <v>2033</v>
-      </c>
-      <c r="U175" s="1">
-        <v>2034</v>
-      </c>
-      <c r="V175" s="1">
-        <v>2035</v>
+      <c r="N175" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:38" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
+        <v>2026</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E176" s="1">
+        <v>1</v>
+      </c>
+      <c r="F176" s="1">
+        <v>1</v>
+      </c>
+      <c r="H176" s="1">
+        <v>1</v>
+      </c>
+      <c r="I176" s="1">
+        <v>1</v>
+      </c>
+      <c r="J176" s="1">
+        <v>1</v>
+      </c>
+      <c r="K176" s="1">
+        <v>1</v>
+      </c>
+      <c r="L176" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>2027</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="E177" s="1">
+        <v>1</v>
+      </c>
+      <c r="F177" s="1">
+        <v>1</v>
+      </c>
+      <c r="O177" s="1">
         <v>2028</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="P177" s="1">
+        <v>2029</v>
+      </c>
+      <c r="Q177" s="1">
+        <v>2030</v>
+      </c>
+      <c r="R177" s="1">
+        <v>2031</v>
+      </c>
+      <c r="S177" s="1">
+        <v>2032</v>
+      </c>
+      <c r="T177" s="1">
+        <v>2033</v>
+      </c>
+      <c r="U177" s="1">
+        <v>2034</v>
+      </c>
+      <c r="V177" s="1">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="178" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>2028</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="C178" s="1" t="s">
         <v>574</v>
-      </c>
-      <c r="E176" s="1">
-        <v>1</v>
-      </c>
-      <c r="F176" s="1">
-        <v>1</v>
-      </c>
-      <c r="H176" s="1">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="1">
-        <v>2029</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="E177" s="1">
-        <v>1</v>
-      </c>
-      <c r="F177" s="1">
-        <v>1</v>
-      </c>
-      <c r="H177" s="1">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="1">
-        <v>2030</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>573</v>
       </c>
       <c r="E178" s="1">
         <v>1</v>
@@ -6624,15 +6643,15 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="E179" s="1">
         <v>1</v>
@@ -6644,100 +6663,140 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
+        <v>2030</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="E180" s="1">
+        <v>1</v>
+      </c>
+      <c r="F180" s="1">
+        <v>1</v>
+      </c>
+      <c r="H180" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>2031</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="E181" s="1">
+        <v>1</v>
+      </c>
+      <c r="F181" s="1">
+        <v>1</v>
+      </c>
+      <c r="H181" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
         <v>2032</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B182" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="C182" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="E180" s="1">
-        <v>1</v>
-      </c>
-      <c r="F180" s="1">
-        <v>1</v>
-      </c>
-      <c r="H180" s="1">
+      <c r="E182" s="1">
+        <v>1</v>
+      </c>
+      <c r="F182" s="1">
+        <v>1</v>
+      </c>
+      <c r="H182" s="1">
         <v>114509</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="1">
+    <row r="183" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
         <v>2033</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B183" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="C183" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="E181" s="1">
-        <v>1</v>
-      </c>
-      <c r="F181" s="1">
-        <v>1</v>
-      </c>
-      <c r="H181" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="1">
+      <c r="E183" s="1">
+        <v>1</v>
+      </c>
+      <c r="F183" s="1">
+        <v>1</v>
+      </c>
+      <c r="H183" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
         <v>2034</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="B184" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="C182" s="1" t="s">
+      <c r="C184" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="E182" s="1">
-        <v>1</v>
-      </c>
-      <c r="F182" s="1">
-        <v>1</v>
-      </c>
-      <c r="H182" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="1">
+      <c r="E184" s="1">
+        <v>1</v>
+      </c>
+      <c r="F184" s="1">
+        <v>1</v>
+      </c>
+      <c r="H184" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
         <v>2035</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="B185" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="C185" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="E183" s="1">
-        <v>1</v>
-      </c>
-      <c r="F183" s="1">
-        <v>1</v>
-      </c>
-      <c r="H183" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="1">
+      <c r="E185" s="1">
+        <v>1</v>
+      </c>
+      <c r="F185" s="1">
+        <v>1</v>
+      </c>
+      <c r="H185" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
         <v>2036</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B186" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="C184" s="1" t="s">
+      <c r="C186" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="E184" s="1">
-        <v>2</v>
-      </c>
-      <c r="F184" s="1">
+      <c r="E186" s="1">
+        <v>2</v>
+      </c>
+      <c r="F186" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>